<commit_message>
runtime update (2025-10-26 22:32:44)
</commit_message>
<xml_diff>
--- a/khl/khl_referees_stats_1369.xlsx
+++ b/khl/khl_referees_stats_1369.xlsx
@@ -1273,7 +1273,7 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -1455,7 +1455,7 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -1819,7 +1819,7 @@
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -1910,7 +1910,7 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -2092,7 +2092,7 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -2183,7 +2183,7 @@
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -3366,7 +3366,7 @@
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -3704,7 +3704,7 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -3795,7 +3795,7 @@
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -3886,7 +3886,7 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -3977,7 +3977,7 @@
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -4068,7 +4068,7 @@
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -4159,7 +4159,7 @@
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -4250,7 +4250,7 @@
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -4341,7 +4341,7 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -4432,7 +4432,7 @@
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -4523,7 +4523,7 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -4614,7 +4614,7 @@
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -4705,7 +4705,7 @@
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -4796,7 +4796,7 @@
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -5069,7 +5069,7 @@
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -5160,7 +5160,7 @@
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -5251,7 +5251,7 @@
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -5342,7 +5342,7 @@
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -5524,7 +5524,7 @@
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -5615,7 +5615,7 @@
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -5706,7 +5706,7 @@
       </c>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -5797,7 +5797,7 @@
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>2025-10-26 10:35:48</t>
+          <t>2025-10-26 14:32:42</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-05 11:03:32)
</commit_message>
<xml_diff>
--- a/khl/khl_referees_stats_1369.xlsx
+++ b/khl/khl_referees_stats_1369.xlsx
@@ -1273,7 +1273,7 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -1455,7 +1455,7 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -1819,7 +1819,7 @@
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -1910,7 +1910,7 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -2092,7 +2092,7 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -2183,7 +2183,7 @@
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -3366,7 +3366,7 @@
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -3704,7 +3704,7 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -3795,7 +3795,7 @@
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -3886,7 +3886,7 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -3977,7 +3977,7 @@
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -4068,7 +4068,7 @@
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -4159,7 +4159,7 @@
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -4250,7 +4250,7 @@
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -4341,7 +4341,7 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -4432,7 +4432,7 @@
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -4523,7 +4523,7 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -4614,7 +4614,7 @@
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -4705,7 +4705,7 @@
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -4796,7 +4796,7 @@
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -5069,7 +5069,7 @@
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -5160,7 +5160,7 @@
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -5251,7 +5251,7 @@
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -5342,7 +5342,7 @@
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -5524,7 +5524,7 @@
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -5615,7 +5615,7 @@
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -5706,7 +5706,7 @@
       </c>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -5797,7 +5797,7 @@
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>2025-11-04 09:23:57</t>
+          <t>2025-11-04 09:58:43</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(runtime): publish files + archive (2025-11-24 08:33:07)
</commit_message>
<xml_diff>
--- a/khl/khl_referees_stats_1369.xlsx
+++ b/khl/khl_referees_stats_1369.xlsx
@@ -1273,7 +1273,7 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -1455,7 +1455,7 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -1819,7 +1819,7 @@
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -1910,7 +1910,7 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -2092,7 +2092,7 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -2183,7 +2183,7 @@
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -3093,7 +3093,7 @@
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -3184,7 +3184,7 @@
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -3366,7 +3366,7 @@
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -3704,7 +3704,7 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -3795,7 +3795,7 @@
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -3886,7 +3886,7 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -3977,7 +3977,7 @@
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -4068,7 +4068,7 @@
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -4159,7 +4159,7 @@
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -4250,7 +4250,7 @@
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -4341,7 +4341,7 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -4432,7 +4432,7 @@
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -4523,7 +4523,7 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -4614,7 +4614,7 @@
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -4705,7 +4705,7 @@
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -4796,7 +4796,7 @@
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="AA16" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -5069,7 +5069,7 @@
       </c>
       <c r="AA17" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -5160,7 +5160,7 @@
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -5251,7 +5251,7 @@
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -5342,7 +5342,7 @@
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -5524,7 +5524,7 @@
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -5615,7 +5615,7 @@
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -5706,7 +5706,7 @@
       </c>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -5797,7 +5797,7 @@
       </c>
       <c r="AA25" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="AA26" t="inlineStr">
         <is>
-          <t>2025-11-23 11:31:32</t>
+          <t>2025-11-23 11:37:25</t>
         </is>
       </c>
     </row>

</xml_diff>